<commit_message>
lower lowerbound to 10e-7
</commit_message>
<xml_diff>
--- a/SDG Financing Simplified model (Egypt)/v4_commented and cleaned - for calibration/input/paraminput_bot.xlsx
+++ b/SDG Financing Simplified model (Egypt)/v4_commented and cleaned - for calibration/input/paraminput_bot.xlsx
@@ -1,17 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Wi2050\SDG Financing Simplified model (Egypt)\v4_commented and cleaned - for calibration\input\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A75E21-1240-4412-B1F1-E9FE37351B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="16160" windowHeight="17780"/>
+    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hardcode" sheetId="2" r:id="rId1"/>
     <sheet name="Continuation" sheetId="3" r:id="rId2"/>
     <sheet name="Index" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -99,361 +115,25 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -476,251 +156,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -728,61 +166,17 @@
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1040,21 +434,21 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.75" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="9" style="1"/>
+    <col min="2" max="2" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1086,7 +480,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>0.074</v>
+        <v>7.3999999999999996E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1102,7 +496,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>0.009</v>
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1110,7 +504,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>0.037</v>
+        <v>3.6999999999999998E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1166,7 +560,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>0.274</v>
+        <v>0.27400000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1174,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>170.472</v>
+        <v>170.47200000000001</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1198,7 +592,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>0.132</v>
+        <v>0.13200000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1206,35 +600,34 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>0.132</v>
-      </c>
-    </row>
-    <row r="20" ht="28.75" spans="1:2">
+        <v>0.13200000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="28.8">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>1e-6</v>
+        <f>10^(-7)</f>
+        <v>9.9999999999999995E-8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="2:2">
+    <row r="1" spans="1:2">
       <c r="B1" t="s">
         <v>20</v>
       </c>
@@ -1402,25 +795,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="19.775" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:5">
+    <row r="1" spans="1:5">
       <c r="D1" t="s">
         <v>21</v>
       </c>
@@ -1455,7 +846,7 @@
         <v>costff</v>
       </c>
       <c r="C3" t="str">
-        <f>IF(B3="","",SUBSTITUTE(SUBSTITUTE(LEFT(_xlfn.FORMULATEXT(B3),FIND("=",_xlfn.FORMULATEXT(B3),2)-1),"=IF(",""),"A","B"))</f>
+        <f ca="1">IF(B3="","",SUBSTITUTE(SUBSTITUTE(LEFT(_xlfn.FORMULATEXT(B3),FIND("=",_xlfn.FORMULATEXT(B3),2)-1),"=IF(",""),"A","B"))</f>
         <v>Hardcode!B1</v>
       </c>
       <c r="D3">
@@ -1477,7 +868,7 @@
         <v>costre</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ref="C4:C67" si="2">IF(B4="","",SUBSTITUTE(SUBSTITUTE(LEFT(_xlfn.FORMULATEXT(B4),FIND("=",_xlfn.FORMULATEXT(B4),2)-1),"=IF(",""),"A","B"))</f>
+        <f t="shared" ref="C4:C67" ca="1" si="2">IF(B4="","",SUBSTITUTE(SUBSTITUTE(LEFT(_xlfn.FORMULATEXT(B4),FIND("=",_xlfn.FORMULATEXT(B4),2)-1),"=IF(",""),"A","B"))</f>
         <v>Hardcode!B2</v>
       </c>
       <c r="D4">
@@ -1499,7 +890,7 @@
         <v>dep</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Hardcode!B3</v>
       </c>
       <c r="D5">
@@ -1521,7 +912,7 @@
         <v>r</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Hardcode!B4</v>
       </c>
       <c r="D6">
@@ -1543,7 +934,7 @@
         <v>kff0</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Hardcode!B5</v>
       </c>
       <c r="D7">
@@ -1565,7 +956,7 @@
         <v>kre0</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Hardcode!B6</v>
       </c>
       <c r="D8">
@@ -1587,7 +978,7 @@
         <v>aff</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Hardcode!B7</v>
       </c>
       <c r="D9">
@@ -1609,7 +1000,7 @@
         <v>taxlim</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Hardcode!B8</v>
       </c>
       <c r="D10">
@@ -1631,7 +1022,7 @@
         <v>tfp1</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Hardcode!B9</v>
       </c>
       <c r="D11">
@@ -1653,7 +1044,7 @@
         <v>phi</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Hardcode!B10</v>
       </c>
       <c r="D12">
@@ -1675,7 +1066,7 @@
         <v>fertsh</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Hardcode!B11</v>
       </c>
       <c r="D13">
@@ -1697,7 +1088,7 @@
         <v>bk</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Hardcode!B12</v>
       </c>
       <c r="D14">
@@ -1719,7 +1110,7 @@
         <v>bkf</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Hardcode!B13</v>
       </c>
       <c r="D15">
@@ -1741,7 +1132,7 @@
         <v>ben</v>
       </c>
       <c r="C16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Hardcode!B14</v>
       </c>
       <c r="D16">
@@ -1763,7 +1154,7 @@
         <v>k0</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Hardcode!B15</v>
       </c>
       <c r="D17">
@@ -1785,7 +1176,7 @@
         <v>kf0</v>
       </c>
       <c r="C18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Hardcode!B16</v>
       </c>
       <c r="D18">
@@ -1807,7 +1198,7 @@
         <v>debtqlim</v>
       </c>
       <c r="C19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Hardcode!B17</v>
       </c>
       <c r="D19">
@@ -1829,7 +1220,7 @@
         <v>gcostsh</v>
       </c>
       <c r="C20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Hardcode!B18</v>
       </c>
       <c r="D20">
@@ -1851,7 +1242,7 @@
         <v>pubgdpsh</v>
       </c>
       <c r="C21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Hardcode!B19</v>
       </c>
       <c r="D21">
@@ -1873,7 +1264,7 @@
         <v>lowerbound</v>
       </c>
       <c r="C22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Hardcode!B20</v>
       </c>
       <c r="D22">
@@ -1895,7 +1286,7 @@
         <v/>
       </c>
       <c r="C23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D23" t="str">
@@ -1917,7 +1308,7 @@
         <v/>
       </c>
       <c r="C24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D24" t="str">
@@ -1939,7 +1330,7 @@
         <v/>
       </c>
       <c r="C25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D25" t="str">
@@ -1961,7 +1352,7 @@
         <v/>
       </c>
       <c r="C26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D26" t="str">
@@ -1983,7 +1374,7 @@
         <v/>
       </c>
       <c r="C27" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D27" t="str">
@@ -2005,7 +1396,7 @@
         <v/>
       </c>
       <c r="C28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D28" t="str">
@@ -2027,7 +1418,7 @@
         <v/>
       </c>
       <c r="C29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D29" t="str">
@@ -2049,7 +1440,7 @@
         <v/>
       </c>
       <c r="C30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D30" t="str">
@@ -2071,7 +1462,7 @@
         <v/>
       </c>
       <c r="C31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D31" t="str">
@@ -2093,7 +1484,7 @@
         <v/>
       </c>
       <c r="C32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D32" t="str">
@@ -2115,7 +1506,7 @@
         <v/>
       </c>
       <c r="C33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D33" t="str">
@@ -2137,7 +1528,7 @@
         <v/>
       </c>
       <c r="C34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D34" t="str">
@@ -2159,7 +1550,7 @@
         <v/>
       </c>
       <c r="C35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D35" t="str">
@@ -2181,7 +1572,7 @@
         <v/>
       </c>
       <c r="C36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D36" t="str">
@@ -2203,7 +1594,7 @@
         <v/>
       </c>
       <c r="C37" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D37" t="str">
@@ -2225,7 +1616,7 @@
         <v/>
       </c>
       <c r="C38" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D38" t="str">
@@ -2247,7 +1638,7 @@
         <v/>
       </c>
       <c r="C39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D39" t="str">
@@ -2269,7 +1660,7 @@
         <v/>
       </c>
       <c r="C40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D40" t="str">
@@ -2291,7 +1682,7 @@
         <v/>
       </c>
       <c r="C41" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D41" t="str">
@@ -2313,7 +1704,7 @@
         <v/>
       </c>
       <c r="C42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D42" t="str">
@@ -2335,7 +1726,7 @@
         <v/>
       </c>
       <c r="C43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D43" t="str">
@@ -2357,7 +1748,7 @@
         <v/>
       </c>
       <c r="C44" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D44" t="str">
@@ -2379,7 +1770,7 @@
         <v/>
       </c>
       <c r="C45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D45" t="str">
@@ -2401,7 +1792,7 @@
         <v/>
       </c>
       <c r="C46" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D46" t="str">
@@ -2423,7 +1814,7 @@
         <v/>
       </c>
       <c r="C47" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D47" t="str">
@@ -2445,7 +1836,7 @@
         <v/>
       </c>
       <c r="C48" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D48" t="str">
@@ -2467,7 +1858,7 @@
         <v/>
       </c>
       <c r="C49" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D49" t="str">
@@ -2489,7 +1880,7 @@
         <v/>
       </c>
       <c r="C50" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D50" t="str">
@@ -2511,7 +1902,7 @@
         <v/>
       </c>
       <c r="C51" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D51" t="str">
@@ -2533,7 +1924,7 @@
         <v/>
       </c>
       <c r="C52" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D52" t="str">
@@ -2555,7 +1946,7 @@
         <v/>
       </c>
       <c r="C53" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D53" t="str">
@@ -2577,7 +1968,7 @@
         <v/>
       </c>
       <c r="C54" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D54" t="str">
@@ -2599,7 +1990,7 @@
         <v/>
       </c>
       <c r="C55" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D55" t="str">
@@ -2621,7 +2012,7 @@
         <v/>
       </c>
       <c r="C56" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D56" t="str">
@@ -2643,7 +2034,7 @@
         <v/>
       </c>
       <c r="C57" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D57" t="str">
@@ -2665,7 +2056,7 @@
         <v/>
       </c>
       <c r="C58" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D58" t="str">
@@ -2687,7 +2078,7 @@
         <v/>
       </c>
       <c r="C59" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D59" t="str">
@@ -2709,7 +2100,7 @@
         <v/>
       </c>
       <c r="C60" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D60" t="str">
@@ -2731,7 +2122,7 @@
         <v/>
       </c>
       <c r="C61" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D61" t="str">
@@ -2753,7 +2144,7 @@
         <v/>
       </c>
       <c r="C62" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D62" t="str">
@@ -2775,7 +2166,7 @@
         <v/>
       </c>
       <c r="C63" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D63" t="str">
@@ -2797,7 +2188,7 @@
         <v/>
       </c>
       <c r="C64" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D64" t="str">
@@ -2819,7 +2210,7 @@
         <v/>
       </c>
       <c r="C65" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D65" t="str">
@@ -2841,7 +2232,7 @@
         <v/>
       </c>
       <c r="C66" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D66" t="str">
@@ -2863,7 +2254,7 @@
         <v/>
       </c>
       <c r="C67" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="D67" t="str">
@@ -2885,7 +2276,7 @@
         <v/>
       </c>
       <c r="C68" t="str">
-        <f t="shared" ref="C68:C101" si="5">IF(B68="","",SUBSTITUTE(SUBSTITUTE(LEFT(_xlfn.FORMULATEXT(B68),FIND("=",_xlfn.FORMULATEXT(B68),2)-1),"=IF(",""),"A","B"))</f>
+        <f t="shared" ref="C68:C101" ca="1" si="5">IF(B68="","",SUBSTITUTE(SUBSTITUTE(LEFT(_xlfn.FORMULATEXT(B68),FIND("=",_xlfn.FORMULATEXT(B68),2)-1),"=IF(",""),"A","B"))</f>
         <v/>
       </c>
       <c r="D68" t="str">
@@ -2907,7 +2298,7 @@
         <v/>
       </c>
       <c r="C69" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D69" t="str">
@@ -2929,7 +2320,7 @@
         <v/>
       </c>
       <c r="C70" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D70" t="str">
@@ -2951,7 +2342,7 @@
         <v/>
       </c>
       <c r="C71" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D71" t="str">
@@ -2973,7 +2364,7 @@
         <v/>
       </c>
       <c r="C72" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D72" t="str">
@@ -2995,7 +2386,7 @@
         <v/>
       </c>
       <c r="C73" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D73" t="str">
@@ -3017,7 +2408,7 @@
         <v/>
       </c>
       <c r="C74" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D74" t="str">
@@ -3039,7 +2430,7 @@
         <v/>
       </c>
       <c r="C75" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D75" t="str">
@@ -3061,7 +2452,7 @@
         <v/>
       </c>
       <c r="C76" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D76" t="str">
@@ -3083,7 +2474,7 @@
         <v/>
       </c>
       <c r="C77" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D77" t="str">
@@ -3105,7 +2496,7 @@
         <v/>
       </c>
       <c r="C78" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D78" t="str">
@@ -3127,7 +2518,7 @@
         <v/>
       </c>
       <c r="C79" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D79" t="str">
@@ -3149,7 +2540,7 @@
         <v/>
       </c>
       <c r="C80" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D80" t="str">
@@ -3171,7 +2562,7 @@
         <v/>
       </c>
       <c r="C81" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D81" t="str">
@@ -3193,7 +2584,7 @@
         <v/>
       </c>
       <c r="C82" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D82" t="str">
@@ -3215,7 +2606,7 @@
         <v/>
       </c>
       <c r="C83" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D83" t="str">
@@ -3237,7 +2628,7 @@
         <v/>
       </c>
       <c r="C84" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D84" t="str">
@@ -3259,7 +2650,7 @@
         <v/>
       </c>
       <c r="C85" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D85" t="str">
@@ -3281,7 +2672,7 @@
         <v/>
       </c>
       <c r="C86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D86" t="str">
@@ -3303,7 +2694,7 @@
         <v/>
       </c>
       <c r="C87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D87" t="str">
@@ -3325,7 +2716,7 @@
         <v/>
       </c>
       <c r="C88" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D88" t="str">
@@ -3347,7 +2738,7 @@
         <v/>
       </c>
       <c r="C89" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D89" t="str">
@@ -3369,7 +2760,7 @@
         <v/>
       </c>
       <c r="C90" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D90" t="str">
@@ -3391,7 +2782,7 @@
         <v/>
       </c>
       <c r="C91" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D91" t="str">
@@ -3413,7 +2804,7 @@
         <v/>
       </c>
       <c r="C92" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D92" t="str">
@@ -3435,7 +2826,7 @@
         <v/>
       </c>
       <c r="C93" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D93" t="str">
@@ -3457,7 +2848,7 @@
         <v/>
       </c>
       <c r="C94" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D94" t="str">
@@ -3479,7 +2870,7 @@
         <v/>
       </c>
       <c r="C95" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D95" t="str">
@@ -3501,7 +2892,7 @@
         <v/>
       </c>
       <c r="C96" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D96" t="str">
@@ -3523,7 +2914,7 @@
         <v/>
       </c>
       <c r="C97" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D97" t="str">
@@ -3545,7 +2936,7 @@
         <v/>
       </c>
       <c r="C98" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D98" t="str">
@@ -3567,7 +2958,7 @@
         <v/>
       </c>
       <c r="C99" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D99" t="str">
@@ -3589,7 +2980,7 @@
         <v/>
       </c>
       <c r="C100" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D100" t="str">
@@ -3611,7 +3002,7 @@
         <v/>
       </c>
       <c r="C101" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="D101" t="str">
@@ -3625,6 +3016,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>